<commit_message>
[RPA Basics] Main에서 모듈 순차 실행 (argument 활용)
</commit_message>
<xml_diff>
--- a/ACME.xlsx
+++ b/ACME.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
   <x:workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ICT CoC\Documents\UiPath\RPA_Lecture\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00706CCB-7BF7-4B62-8AE9-D9F16CCA0C48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView firstSheet="0" activeTab="0"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7845" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="WI_원본" sheetId="2" r:id="rId2"/>
-    <x:sheet name="WI_가공" sheetId="5" r:id="rId5"/>
+    <x:sheet name="Sheet1" sheetId="8" r:id="rId1"/>
+    <x:sheet name="WI_원본" sheetId="4" r:id="rId4"/>
+    <x:sheet name="WI_가공" sheetId="6" r:id="rId6"/>
+    <x:sheet name="WI_가공_세부" sheetId="7" r:id="rId7"/>
+    <x:sheet name="RPA수행결과" sheetId="9" r:id="rId9"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="125725"/>
+  <x:calcPr calcId="0"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="436">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="502">
   <x:si>
     <x:t>Actions</x:t>
   </x:si>
@@ -50,24 +60,27 @@
     <x:t>WI5</x:t>
   </x:si>
   <x:si>
+    <x:t>Completed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2023-05-05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://acme-test.uipath.com/work-items/100629894</x:t>
+  </x:si>
+  <x:si>
+    <x:t>100629894</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Research Client Check Copy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WI2</x:t>
+  </x:si>
+  <x:si>
     <x:t>Open</x:t>
   </x:si>
   <x:si>
-    <x:t>2023-05-05</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://acme-test.uipath.com/work-items/100629894</x:t>
-  </x:si>
-  <x:si>
-    <x:t>100629894</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Research Client Check Copy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>WI2</x:t>
-  </x:si>
-  <x:si>
     <x:t>2021-12-28</x:t>
   </x:si>
   <x:si>
@@ -1323,22 +1336,222 @@
   </x:si>
   <x:si>
     <x:t>Client Country</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hash</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NU74295</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tiny Erhart</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Romania</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4882ebf8c03df53c30e512a49d681b132b0a38eb</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EU67601</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Floy Shedd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>France</x:t>
+  </x:si>
+  <x:si>
+    <x:t>b2c37847cdd619e4eb57091d1cbd8cac6e9b03a6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KI44163</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Edison Byam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Germany</x:t>
+  </x:si>
+  <x:si>
+    <x:t>eda668adbed17c579e580282b6e5b1a72700acbf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AZ79829</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Marylou Kenworthy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Italy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>07e7c66179907494b3c4fbcadcc5bfc0c2399550</x:t>
+  </x:si>
+  <x:si>
+    <x:t>XW47730</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shanita Plumber</x:t>
+  </x:si>
+  <x:si>
+    <x:t>43b4a48c73a95106f8f5b6eaaeb61b0142b73df2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FP75053</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bud Baril</x:t>
+  </x:si>
+  <x:si>
+    <x:t>c641355d0f7fafdd6037fb19303c8363794c6ae3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KJ93404</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Garret Reising</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dafc9516e64e98e9bfd379d9e5b26e77f715cfcb</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BL17488</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mabel Suttle</x:t>
+  </x:si>
+  <x:si>
+    <x:t>94ac0eb0dce0fbe7548eafb7a93342ff51470346</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DB83622</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wilson Gau</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7b3377d3426500876741838c26f83b332c54f4c0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CX76110</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mirian Derosier</x:t>
+  </x:si>
+  <x:si>
+    <x:t>f2a6a7a06026ac3d05b6b84c93505b23cb23d303</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RU90268</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Veda Blaylock</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9b706d312182d6588267c852c9d5ecfc22208d34</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RW82952</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jesica Rutt</x:t>
+  </x:si>
+  <x:si>
+    <x:t>88872ad53682de9e00c72c54e72a5ceda130f5d6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UK18656</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Raymond Crider</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30d95d99ad2c100c596bddbac7880773896f82be</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AD88069</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Craig Tober</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1c514c4689f77b487ebcebb3a092bbbff02c7fef</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FT44139</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Allan Camara</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ce2df4044c200f94c8dcdb14e9a1191085fc912a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>QS86336</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Donn Chabot</x:t>
+  </x:si>
+  <x:si>
+    <x:t>d408e344ca46072d44f04befc0a9c4efe7dbf256</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PO26319</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Normand Bently</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4b689b8903814a74ccae87c1ae4453ee01560ec1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OZ56329</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Anna Dudas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7cc4773d7fa298cab1f5c637d00bca23e187d67b</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FY17206</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bradford Cleaver</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7da2444497b885594cd80f066454d5d9e349f78a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HT69354</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hilario Weitzel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>96808e6572a5befff0508e654d8b42537b0aaabe</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="2" x14ac:knownFonts="1">
     <x:font>
-      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
       <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:sz val="8"/>
+      <x:name val="돋움"/>
+      <x:family val="3"/>
+      <x:charset val="129"/>
     </x:font>
   </x:fonts>
   <x:fills count="2">
@@ -1350,38 +1563,32 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </x:cellStyleXfs>
   <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </x:cellXfs>
   <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <x:cellStyle name="표준" xfId="0" builtinId="0"/>
   </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </x:ext>
+  </x:extLst>
 </x:styleSheet>
 </file>
 
@@ -1669,6 +1876,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{A9A2B387-96FC-4E8E-AAED-6077339EB555}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData/>
+  <x:phoneticPr fontId="1" type="noConversion"/>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="9" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1736,78 +1963,78 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G3" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:7">
       <x:c r="B4" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G4" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:7">
       <x:c r="B5" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:7">
       <x:c r="B6" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:7">
       <x:c r="B7" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
         <x:v>15</x:v>
@@ -1816,38 +2043,38 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:7">
       <x:c r="B8" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G8" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:7">
       <x:c r="B9" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
         <x:v>15</x:v>
@@ -1856,18 +2083,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:7">
       <x:c r="B10" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
         <x:v>15</x:v>
@@ -1876,18 +2103,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:7">
       <x:c r="B11" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
         <x:v>15</x:v>
@@ -1896,38 +2123,38 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:7">
       <x:c r="B12" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F12" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:7">
       <x:c r="B13" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
         <x:v>15</x:v>
@@ -1936,18 +2163,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F13" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:7">
       <x:c r="B14" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
         <x:v>15</x:v>
@@ -1956,78 +2183,78 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F14" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:7">
       <x:c r="B15" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F15" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G15" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:7">
       <x:c r="B16" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F16" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G16" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:7">
       <x:c r="B17" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E17" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F17" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G17" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:7">
       <x:c r="B18" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
         <x:v>15</x:v>
@@ -2036,38 +2263,38 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F18" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G18" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:7">
       <x:c r="B19" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F19" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G19" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:7">
       <x:c r="B20" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
         <x:v>15</x:v>
@@ -2076,18 +2303,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F20" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G20" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:7">
       <x:c r="B21" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
         <x:v>9</x:v>
@@ -2099,15 +2326,15 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G21" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:7">
       <x:c r="B22" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
         <x:v>9</x:v>
@@ -2119,15 +2346,15 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G22" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:7">
       <x:c r="B23" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
         <x:v>9</x:v>
@@ -2139,55 +2366,55 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G23" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:7">
       <x:c r="B24" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E24" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F24" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G24" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:7">
       <x:c r="B25" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E25" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F25" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G25" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:7">
       <x:c r="B26" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
         <x:v>15</x:v>
@@ -2196,98 +2423,98 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F26" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G26" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:7">
       <x:c r="B27" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="C27" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="D27" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E27" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F27" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G27" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:7">
       <x:c r="B28" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="D28" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E28" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F28" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G28" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:7">
       <x:c r="B29" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="D29" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E29" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F29" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G29" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:7">
       <x:c r="B30" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="C30" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="D30" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E30" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F30" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G30" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:7">
       <x:c r="B31" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="C31" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="D31" s="0" t="s">
         <x:v>15</x:v>
@@ -2296,38 +2523,38 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F31" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G31" s="0" t="s">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:7">
       <x:c r="B32" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C32" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="D32" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E32" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F32" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G32" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:7">
       <x:c r="B33" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="C33" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="D33" s="0" t="s">
         <x:v>15</x:v>
@@ -2336,18 +2563,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F33" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G33" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:7">
       <x:c r="B34" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C34" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="D34" s="0" t="s">
         <x:v>15</x:v>
@@ -2356,38 +2583,38 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F34" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G34" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:7">
       <x:c r="B35" s="0" t="s">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="C35" s="0" t="s">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="D35" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E35" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F35" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G35" s="0" t="s">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:7">
       <x:c r="B36" s="0" t="s">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="C36" s="0" t="s">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="D36" s="0" t="s">
         <x:v>15</x:v>
@@ -2396,18 +2623,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F36" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G36" s="0" t="s">
-        <x:v>121</x:v>
+        <x:v>122</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:7">
       <x:c r="B37" s="0" t="s">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="C37" s="0" t="s">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="D37" s="0" t="s">
         <x:v>15</x:v>
@@ -2416,18 +2643,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F37" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G37" s="0" t="s">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:7">
       <x:c r="B38" s="0" t="s">
-        <x:v>125</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="C38" s="0" t="s">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="D38" s="0" t="s">
         <x:v>15</x:v>
@@ -2436,38 +2663,38 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F38" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G38" s="0" t="s">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:7">
       <x:c r="B39" s="0" t="s">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="C39" s="0" t="s">
-        <x:v>129</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="D39" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E39" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F39" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G39" s="0" t="s">
-        <x:v>130</x:v>
+        <x:v>131</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:7">
       <x:c r="B40" s="0" t="s">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="C40" s="0" t="s">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="D40" s="0" t="s">
         <x:v>15</x:v>
@@ -2476,38 +2703,38 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F40" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G40" s="0" t="s">
-        <x:v>133</x:v>
+        <x:v>134</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:7">
       <x:c r="B41" s="0" t="s">
-        <x:v>134</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="C41" s="0" t="s">
-        <x:v>135</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="D41" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E41" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F41" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G41" s="0" t="s">
-        <x:v>136</x:v>
+        <x:v>137</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:7">
       <x:c r="B42" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="C42" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="D42" s="0" t="s">
         <x:v>9</x:v>
@@ -2519,35 +2746,35 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G42" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:7">
       <x:c r="B43" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="C43" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="D43" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E43" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F43" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G43" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>143</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:7">
       <x:c r="B44" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="C44" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="D44" s="0" t="s">
         <x:v>9</x:v>
@@ -2559,15 +2786,15 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G44" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>146</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:7">
       <x:c r="B45" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="C45" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="D45" s="0" t="s">
         <x:v>9</x:v>
@@ -2579,35 +2806,35 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G45" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:7">
       <x:c r="B46" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="C46" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="D46" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E46" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F46" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G46" s="0" t="s">
-        <x:v>151</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:7">
       <x:c r="B47" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="C47" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="D47" s="0" t="s">
         <x:v>15</x:v>
@@ -2616,38 +2843,38 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F47" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G47" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>155</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:7">
       <x:c r="B48" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="C48" s="0" t="s">
-        <x:v>156</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="D48" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E48" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F48" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G48" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>158</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:7">
       <x:c r="B49" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="C49" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="D49" s="0" t="s">
         <x:v>15</x:v>
@@ -2656,38 +2883,38 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F49" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G49" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>161</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:7">
       <x:c r="B50" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="C50" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="D50" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E50" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F50" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G50" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>164</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:7">
       <x:c r="B51" s="0" t="s">
-        <x:v>164</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="C51" s="0" t="s">
-        <x:v>165</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="D51" s="0" t="s">
         <x:v>15</x:v>
@@ -2696,18 +2923,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F51" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G51" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>167</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:7">
       <x:c r="B52" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="C52" s="0" t="s">
-        <x:v>168</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="D52" s="0" t="s">
         <x:v>15</x:v>
@@ -2716,18 +2943,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F52" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G52" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>170</x:v>
       </x:c>
     </x:row>
     <x:row r="53" spans="1:7">
       <x:c r="B53" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="C53" s="0" t="s">
-        <x:v>171</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="D53" s="0" t="s">
         <x:v>15</x:v>
@@ -2736,78 +2963,78 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F53" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G53" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>173</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:7">
       <x:c r="B54" s="0" t="s">
-        <x:v>173</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="C54" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="D54" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E54" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F54" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G54" s="0" t="s">
-        <x:v>175</x:v>
+        <x:v>176</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:7">
       <x:c r="B55" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="C55" s="0" t="s">
-        <x:v>177</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="D55" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E55" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F55" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G55" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>179</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:7">
       <x:c r="B56" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="C56" s="0" t="s">
-        <x:v>180</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="D56" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E56" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F56" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G56" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>182</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:7">
       <x:c r="B57" s="0" t="s">
-        <x:v>182</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="C57" s="0" t="s">
-        <x:v>183</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="D57" s="0" t="s">
         <x:v>15</x:v>
@@ -2816,18 +3043,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F57" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G57" s="0" t="s">
-        <x:v>184</x:v>
+        <x:v>185</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:7">
       <x:c r="B58" s="0" t="s">
-        <x:v>185</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="C58" s="0" t="s">
-        <x:v>186</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="D58" s="0" t="s">
         <x:v>15</x:v>
@@ -2836,18 +3063,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F58" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G58" s="0" t="s">
-        <x:v>187</x:v>
+        <x:v>188</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:7">
       <x:c r="B59" s="0" t="s">
-        <x:v>188</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="C59" s="0" t="s">
-        <x:v>189</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="D59" s="0" t="s">
         <x:v>15</x:v>
@@ -2856,98 +3083,98 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F59" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G59" s="0" t="s">
-        <x:v>190</x:v>
+        <x:v>191</x:v>
       </x:c>
     </x:row>
     <x:row r="60" spans="1:7">
       <x:c r="B60" s="0" t="s">
-        <x:v>191</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="C60" s="0" t="s">
-        <x:v>192</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="D60" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E60" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F60" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G60" s="0" t="s">
-        <x:v>193</x:v>
+        <x:v>194</x:v>
       </x:c>
     </x:row>
     <x:row r="61" spans="1:7">
       <x:c r="B61" s="0" t="s">
-        <x:v>194</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="C61" s="0" t="s">
-        <x:v>195</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="D61" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E61" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F61" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G61" s="0" t="s">
-        <x:v>196</x:v>
+        <x:v>197</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:7">
       <x:c r="B62" s="0" t="s">
-        <x:v>197</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="C62" s="0" t="s">
-        <x:v>198</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="D62" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E62" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F62" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G62" s="0" t="s">
-        <x:v>199</x:v>
+        <x:v>200</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:7">
       <x:c r="B63" s="0" t="s">
-        <x:v>200</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="C63" s="0" t="s">
-        <x:v>201</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="D63" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E63" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F63" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G63" s="0" t="s">
-        <x:v>202</x:v>
+        <x:v>203</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:7">
       <x:c r="B64" s="0" t="s">
-        <x:v>203</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="C64" s="0" t="s">
-        <x:v>204</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="D64" s="0" t="s">
         <x:v>15</x:v>
@@ -2956,18 +3183,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F64" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G64" s="0" t="s">
-        <x:v>205</x:v>
+        <x:v>206</x:v>
       </x:c>
     </x:row>
     <x:row r="65" spans="1:7">
       <x:c r="B65" s="0" t="s">
-        <x:v>206</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="C65" s="0" t="s">
-        <x:v>207</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="D65" s="0" t="s">
         <x:v>15</x:v>
@@ -2976,18 +3203,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F65" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G65" s="0" t="s">
-        <x:v>208</x:v>
+        <x:v>209</x:v>
       </x:c>
     </x:row>
     <x:row r="66" spans="1:7">
       <x:c r="B66" s="0" t="s">
-        <x:v>209</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="C66" s="0" t="s">
-        <x:v>210</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="D66" s="0" t="s">
         <x:v>15</x:v>
@@ -2996,98 +3223,98 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F66" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G66" s="0" t="s">
-        <x:v>211</x:v>
+        <x:v>212</x:v>
       </x:c>
     </x:row>
     <x:row r="67" spans="1:7">
       <x:c r="B67" s="0" t="s">
-        <x:v>212</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="C67" s="0" t="s">
-        <x:v>213</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="D67" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E67" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F67" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G67" s="0" t="s">
-        <x:v>214</x:v>
+        <x:v>215</x:v>
       </x:c>
     </x:row>
     <x:row r="68" spans="1:7">
       <x:c r="B68" s="0" t="s">
-        <x:v>215</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="C68" s="0" t="s">
-        <x:v>216</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="D68" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E68" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F68" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G68" s="0" t="s">
-        <x:v>217</x:v>
+        <x:v>218</x:v>
       </x:c>
     </x:row>
     <x:row r="69" spans="1:7">
       <x:c r="B69" s="0" t="s">
-        <x:v>218</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="C69" s="0" t="s">
-        <x:v>219</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="D69" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E69" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F69" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G69" s="0" t="s">
-        <x:v>220</x:v>
+        <x:v>221</x:v>
       </x:c>
     </x:row>
     <x:row r="70" spans="1:7">
       <x:c r="B70" s="0" t="s">
-        <x:v>221</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="C70" s="0" t="s">
-        <x:v>222</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="D70" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E70" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F70" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G70" s="0" t="s">
-        <x:v>223</x:v>
+        <x:v>224</x:v>
       </x:c>
     </x:row>
     <x:row r="71" spans="1:7">
       <x:c r="B71" s="0" t="s">
-        <x:v>224</x:v>
+        <x:v>225</x:v>
       </x:c>
       <x:c r="C71" s="0" t="s">
-        <x:v>225</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="D71" s="0" t="s">
         <x:v>15</x:v>
@@ -3096,118 +3323,118 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F71" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G71" s="0" t="s">
-        <x:v>226</x:v>
+        <x:v>227</x:v>
       </x:c>
     </x:row>
     <x:row r="72" spans="1:7">
       <x:c r="B72" s="0" t="s">
-        <x:v>227</x:v>
+        <x:v>228</x:v>
       </x:c>
       <x:c r="C72" s="0" t="s">
-        <x:v>228</x:v>
+        <x:v>229</x:v>
       </x:c>
       <x:c r="D72" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E72" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F72" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G72" s="0" t="s">
-        <x:v>229</x:v>
+        <x:v>230</x:v>
       </x:c>
     </x:row>
     <x:row r="73" spans="1:7">
       <x:c r="B73" s="0" t="s">
-        <x:v>230</x:v>
+        <x:v>231</x:v>
       </x:c>
       <x:c r="C73" s="0" t="s">
-        <x:v>231</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="D73" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E73" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F73" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G73" s="0" t="s">
-        <x:v>232</x:v>
+        <x:v>233</x:v>
       </x:c>
     </x:row>
     <x:row r="74" spans="1:7">
       <x:c r="B74" s="0" t="s">
-        <x:v>233</x:v>
+        <x:v>234</x:v>
       </x:c>
       <x:c r="C74" s="0" t="s">
-        <x:v>234</x:v>
+        <x:v>235</x:v>
       </x:c>
       <x:c r="D74" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E74" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F74" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G74" s="0" t="s">
-        <x:v>235</x:v>
+        <x:v>236</x:v>
       </x:c>
     </x:row>
     <x:row r="75" spans="1:7">
       <x:c r="B75" s="0" t="s">
-        <x:v>236</x:v>
+        <x:v>237</x:v>
       </x:c>
       <x:c r="C75" s="0" t="s">
-        <x:v>237</x:v>
+        <x:v>238</x:v>
       </x:c>
       <x:c r="D75" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E75" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F75" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G75" s="0" t="s">
-        <x:v>238</x:v>
+        <x:v>239</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="1:7">
       <x:c r="B76" s="0" t="s">
-        <x:v>239</x:v>
+        <x:v>240</x:v>
       </x:c>
       <x:c r="C76" s="0" t="s">
-        <x:v>240</x:v>
+        <x:v>241</x:v>
       </x:c>
       <x:c r="D76" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E76" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F76" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G76" s="0" t="s">
-        <x:v>241</x:v>
+        <x:v>242</x:v>
       </x:c>
     </x:row>
     <x:row r="77" spans="1:7">
       <x:c r="B77" s="0" t="s">
-        <x:v>242</x:v>
+        <x:v>243</x:v>
       </x:c>
       <x:c r="C77" s="0" t="s">
-        <x:v>243</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="D77" s="0" t="s">
         <x:v>15</x:v>
@@ -3216,18 +3443,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F77" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G77" s="0" t="s">
-        <x:v>244</x:v>
+        <x:v>245</x:v>
       </x:c>
     </x:row>
     <x:row r="78" spans="1:7">
       <x:c r="B78" s="0" t="s">
-        <x:v>245</x:v>
+        <x:v>246</x:v>
       </x:c>
       <x:c r="C78" s="0" t="s">
-        <x:v>246</x:v>
+        <x:v>247</x:v>
       </x:c>
       <x:c r="D78" s="0" t="s">
         <x:v>15</x:v>
@@ -3236,58 +3463,58 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F78" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G78" s="0" t="s">
-        <x:v>247</x:v>
+        <x:v>248</x:v>
       </x:c>
     </x:row>
     <x:row r="79" spans="1:7">
       <x:c r="B79" s="0" t="s">
-        <x:v>248</x:v>
+        <x:v>249</x:v>
       </x:c>
       <x:c r="C79" s="0" t="s">
-        <x:v>249</x:v>
+        <x:v>250</x:v>
       </x:c>
       <x:c r="D79" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E79" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F79" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G79" s="0" t="s">
-        <x:v>250</x:v>
+        <x:v>251</x:v>
       </x:c>
     </x:row>
     <x:row r="80" spans="1:7">
       <x:c r="B80" s="0" t="s">
-        <x:v>251</x:v>
+        <x:v>252</x:v>
       </x:c>
       <x:c r="C80" s="0" t="s">
-        <x:v>252</x:v>
+        <x:v>253</x:v>
       </x:c>
       <x:c r="D80" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E80" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F80" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G80" s="0" t="s">
-        <x:v>253</x:v>
+        <x:v>254</x:v>
       </x:c>
     </x:row>
     <x:row r="81" spans="1:7">
       <x:c r="B81" s="0" t="s">
-        <x:v>254</x:v>
+        <x:v>255</x:v>
       </x:c>
       <x:c r="C81" s="0" t="s">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="D81" s="0" t="s">
         <x:v>9</x:v>
@@ -3299,35 +3526,35 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G81" s="0" t="s">
-        <x:v>256</x:v>
+        <x:v>257</x:v>
       </x:c>
     </x:row>
     <x:row r="82" spans="1:7">
       <x:c r="B82" s="0" t="s">
-        <x:v>257</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="C82" s="0" t="s">
-        <x:v>258</x:v>
+        <x:v>259</x:v>
       </x:c>
       <x:c r="D82" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E82" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F82" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G82" s="0" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:7">
       <x:c r="B83" s="0" t="s">
-        <x:v>260</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="C83" s="0" t="s">
-        <x:v>261</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="D83" s="0" t="s">
         <x:v>9</x:v>
@@ -3339,35 +3566,35 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G83" s="0" t="s">
-        <x:v>262</x:v>
+        <x:v>263</x:v>
       </x:c>
     </x:row>
     <x:row r="84" spans="1:7">
       <x:c r="B84" s="0" t="s">
-        <x:v>263</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="C84" s="0" t="s">
-        <x:v>264</x:v>
+        <x:v>265</x:v>
       </x:c>
       <x:c r="D84" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E84" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F84" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G84" s="0" t="s">
-        <x:v>265</x:v>
+        <x:v>266</x:v>
       </x:c>
     </x:row>
     <x:row r="85" spans="1:7">
       <x:c r="B85" s="0" t="s">
-        <x:v>266</x:v>
+        <x:v>267</x:v>
       </x:c>
       <x:c r="C85" s="0" t="s">
-        <x:v>267</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="D85" s="0" t="s">
         <x:v>15</x:v>
@@ -3376,98 +3603,98 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F85" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G85" s="0" t="s">
-        <x:v>268</x:v>
+        <x:v>269</x:v>
       </x:c>
     </x:row>
     <x:row r="86" spans="1:7">
       <x:c r="B86" s="0" t="s">
-        <x:v>269</x:v>
+        <x:v>270</x:v>
       </x:c>
       <x:c r="C86" s="0" t="s">
-        <x:v>270</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="D86" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E86" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F86" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G86" s="0" t="s">
-        <x:v>271</x:v>
+        <x:v>272</x:v>
       </x:c>
     </x:row>
     <x:row r="87" spans="1:7">
       <x:c r="B87" s="0" t="s">
-        <x:v>272</x:v>
+        <x:v>273</x:v>
       </x:c>
       <x:c r="C87" s="0" t="s">
-        <x:v>273</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="D87" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E87" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F87" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G87" s="0" t="s">
-        <x:v>274</x:v>
+        <x:v>275</x:v>
       </x:c>
     </x:row>
     <x:row r="88" spans="1:7">
       <x:c r="B88" s="0" t="s">
-        <x:v>275</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="C88" s="0" t="s">
-        <x:v>276</x:v>
+        <x:v>277</x:v>
       </x:c>
       <x:c r="D88" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E88" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F88" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G88" s="0" t="s">
-        <x:v>277</x:v>
+        <x:v>278</x:v>
       </x:c>
     </x:row>
     <x:row r="89" spans="1:7">
       <x:c r="B89" s="0" t="s">
-        <x:v>278</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="C89" s="0" t="s">
-        <x:v>279</x:v>
+        <x:v>280</x:v>
       </x:c>
       <x:c r="D89" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E89" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F89" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G89" s="0" t="s">
-        <x:v>280</x:v>
+        <x:v>281</x:v>
       </x:c>
     </x:row>
     <x:row r="90" spans="1:7">
       <x:c r="B90" s="0" t="s">
-        <x:v>281</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="C90" s="0" t="s">
-        <x:v>282</x:v>
+        <x:v>283</x:v>
       </x:c>
       <x:c r="D90" s="0" t="s">
         <x:v>15</x:v>
@@ -3476,18 +3703,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F90" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G90" s="0" t="s">
-        <x:v>283</x:v>
+        <x:v>284</x:v>
       </x:c>
     </x:row>
     <x:row r="91" spans="1:7">
       <x:c r="B91" s="0" t="s">
-        <x:v>284</x:v>
+        <x:v>285</x:v>
       </x:c>
       <x:c r="C91" s="0" t="s">
-        <x:v>285</x:v>
+        <x:v>286</x:v>
       </x:c>
       <x:c r="D91" s="0" t="s">
         <x:v>15</x:v>
@@ -3496,18 +3723,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F91" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G91" s="0" t="s">
-        <x:v>286</x:v>
+        <x:v>287</x:v>
       </x:c>
     </x:row>
     <x:row r="92" spans="1:7">
       <x:c r="B92" s="0" t="s">
-        <x:v>287</x:v>
+        <x:v>288</x:v>
       </x:c>
       <x:c r="C92" s="0" t="s">
-        <x:v>288</x:v>
+        <x:v>289</x:v>
       </x:c>
       <x:c r="D92" s="0" t="s">
         <x:v>15</x:v>
@@ -3516,38 +3743,38 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F92" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G92" s="0" t="s">
-        <x:v>289</x:v>
+        <x:v>290</x:v>
       </x:c>
     </x:row>
     <x:row r="93" spans="1:7">
       <x:c r="B93" s="0" t="s">
-        <x:v>290</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="C93" s="0" t="s">
-        <x:v>291</x:v>
+        <x:v>292</x:v>
       </x:c>
       <x:c r="D93" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E93" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F93" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G93" s="0" t="s">
-        <x:v>292</x:v>
+        <x:v>293</x:v>
       </x:c>
     </x:row>
     <x:row r="94" spans="1:7">
       <x:c r="B94" s="0" t="s">
-        <x:v>293</x:v>
+        <x:v>294</x:v>
       </x:c>
       <x:c r="C94" s="0" t="s">
-        <x:v>294</x:v>
+        <x:v>295</x:v>
       </x:c>
       <x:c r="D94" s="0" t="s">
         <x:v>15</x:v>
@@ -3556,18 +3783,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F94" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G94" s="0" t="s">
-        <x:v>295</x:v>
+        <x:v>296</x:v>
       </x:c>
     </x:row>
     <x:row r="95" spans="1:7">
       <x:c r="B95" s="0" t="s">
-        <x:v>296</x:v>
+        <x:v>297</x:v>
       </x:c>
       <x:c r="C95" s="0" t="s">
-        <x:v>297</x:v>
+        <x:v>298</x:v>
       </x:c>
       <x:c r="D95" s="0" t="s">
         <x:v>9</x:v>
@@ -3579,35 +3806,35 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G95" s="0" t="s">
-        <x:v>298</x:v>
+        <x:v>299</x:v>
       </x:c>
     </x:row>
     <x:row r="96" spans="1:7">
       <x:c r="B96" s="0" t="s">
-        <x:v>299</x:v>
+        <x:v>300</x:v>
       </x:c>
       <x:c r="C96" s="0" t="s">
-        <x:v>300</x:v>
+        <x:v>301</x:v>
       </x:c>
       <x:c r="D96" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E96" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F96" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G96" s="0" t="s">
-        <x:v>301</x:v>
+        <x:v>302</x:v>
       </x:c>
     </x:row>
     <x:row r="97" spans="1:7">
       <x:c r="B97" s="0" t="s">
-        <x:v>302</x:v>
+        <x:v>303</x:v>
       </x:c>
       <x:c r="C97" s="0" t="s">
-        <x:v>303</x:v>
+        <x:v>304</x:v>
       </x:c>
       <x:c r="D97" s="0" t="s">
         <x:v>9</x:v>
@@ -3619,35 +3846,35 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G97" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>305</x:v>
       </x:c>
     </x:row>
     <x:row r="98" spans="1:7">
       <x:c r="B98" s="0" t="s">
-        <x:v>305</x:v>
+        <x:v>306</x:v>
       </x:c>
       <x:c r="C98" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>307</x:v>
       </x:c>
       <x:c r="D98" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E98" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F98" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G98" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>308</x:v>
       </x:c>
     </x:row>
     <x:row r="99" spans="1:7">
       <x:c r="B99" s="0" t="s">
-        <x:v>308</x:v>
+        <x:v>309</x:v>
       </x:c>
       <x:c r="C99" s="0" t="s">
-        <x:v>309</x:v>
+        <x:v>310</x:v>
       </x:c>
       <x:c r="D99" s="0" t="s">
         <x:v>15</x:v>
@@ -3656,18 +3883,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F99" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G99" s="0" t="s">
-        <x:v>310</x:v>
+        <x:v>311</x:v>
       </x:c>
     </x:row>
     <x:row r="100" spans="1:7">
       <x:c r="B100" s="0" t="s">
-        <x:v>311</x:v>
+        <x:v>312</x:v>
       </x:c>
       <x:c r="C100" s="0" t="s">
-        <x:v>312</x:v>
+        <x:v>313</x:v>
       </x:c>
       <x:c r="D100" s="0" t="s">
         <x:v>15</x:v>
@@ -3676,38 +3903,38 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F100" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G100" s="0" t="s">
-        <x:v>313</x:v>
+        <x:v>314</x:v>
       </x:c>
     </x:row>
     <x:row r="101" spans="1:7">
       <x:c r="B101" s="0" t="s">
-        <x:v>314</x:v>
+        <x:v>315</x:v>
       </x:c>
       <x:c r="C101" s="0" t="s">
-        <x:v>315</x:v>
+        <x:v>316</x:v>
       </x:c>
       <x:c r="D101" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E101" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F101" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G101" s="0" t="s">
-        <x:v>316</x:v>
+        <x:v>317</x:v>
       </x:c>
     </x:row>
     <x:row r="102" spans="1:7">
       <x:c r="B102" s="0" t="s">
-        <x:v>317</x:v>
+        <x:v>318</x:v>
       </x:c>
       <x:c r="C102" s="0" t="s">
-        <x:v>318</x:v>
+        <x:v>319</x:v>
       </x:c>
       <x:c r="D102" s="0" t="s">
         <x:v>15</x:v>
@@ -3716,18 +3943,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F102" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G102" s="0" t="s">
-        <x:v>319</x:v>
+        <x:v>320</x:v>
       </x:c>
     </x:row>
     <x:row r="103" spans="1:7">
       <x:c r="B103" s="0" t="s">
-        <x:v>320</x:v>
+        <x:v>321</x:v>
       </x:c>
       <x:c r="C103" s="0" t="s">
-        <x:v>321</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="D103" s="0" t="s">
         <x:v>9</x:v>
@@ -3739,35 +3966,35 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G103" s="0" t="s">
-        <x:v>322</x:v>
+        <x:v>323</x:v>
       </x:c>
     </x:row>
     <x:row r="104" spans="1:7">
       <x:c r="B104" s="0" t="s">
-        <x:v>323</x:v>
+        <x:v>324</x:v>
       </x:c>
       <x:c r="C104" s="0" t="s">
-        <x:v>324</x:v>
+        <x:v>325</x:v>
       </x:c>
       <x:c r="D104" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E104" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F104" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G104" s="0" t="s">
-        <x:v>325</x:v>
+        <x:v>326</x:v>
       </x:c>
     </x:row>
     <x:row r="105" spans="1:7">
       <x:c r="B105" s="0" t="s">
-        <x:v>326</x:v>
+        <x:v>327</x:v>
       </x:c>
       <x:c r="C105" s="0" t="s">
-        <x:v>327</x:v>
+        <x:v>328</x:v>
       </x:c>
       <x:c r="D105" s="0" t="s">
         <x:v>9</x:v>
@@ -3779,35 +4006,35 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G105" s="0" t="s">
-        <x:v>328</x:v>
+        <x:v>329</x:v>
       </x:c>
     </x:row>
     <x:row r="106" spans="1:7">
       <x:c r="B106" s="0" t="s">
-        <x:v>329</x:v>
+        <x:v>330</x:v>
       </x:c>
       <x:c r="C106" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>331</x:v>
       </x:c>
       <x:c r="D106" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E106" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F106" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G106" s="0" t="s">
-        <x:v>331</x:v>
+        <x:v>332</x:v>
       </x:c>
     </x:row>
     <x:row r="107" spans="1:7">
       <x:c r="B107" s="0" t="s">
-        <x:v>332</x:v>
+        <x:v>333</x:v>
       </x:c>
       <x:c r="C107" s="0" t="s">
-        <x:v>333</x:v>
+        <x:v>334</x:v>
       </x:c>
       <x:c r="D107" s="0" t="s">
         <x:v>9</x:v>
@@ -3819,15 +4046,15 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G107" s="0" t="s">
-        <x:v>334</x:v>
+        <x:v>335</x:v>
       </x:c>
     </x:row>
     <x:row r="108" spans="1:7">
       <x:c r="B108" s="0" t="s">
-        <x:v>335</x:v>
+        <x:v>336</x:v>
       </x:c>
       <x:c r="C108" s="0" t="s">
-        <x:v>336</x:v>
+        <x:v>337</x:v>
       </x:c>
       <x:c r="D108" s="0" t="s">
         <x:v>9</x:v>
@@ -3839,15 +4066,15 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G108" s="0" t="s">
-        <x:v>337</x:v>
+        <x:v>338</x:v>
       </x:c>
     </x:row>
     <x:row r="109" spans="1:7">
       <x:c r="B109" s="0" t="s">
-        <x:v>338</x:v>
+        <x:v>339</x:v>
       </x:c>
       <x:c r="C109" s="0" t="s">
-        <x:v>339</x:v>
+        <x:v>340</x:v>
       </x:c>
       <x:c r="D109" s="0" t="s">
         <x:v>15</x:v>
@@ -3856,18 +4083,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F109" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G109" s="0" t="s">
-        <x:v>340</x:v>
+        <x:v>341</x:v>
       </x:c>
     </x:row>
     <x:row r="110" spans="1:7">
       <x:c r="B110" s="0" t="s">
-        <x:v>341</x:v>
+        <x:v>342</x:v>
       </x:c>
       <x:c r="C110" s="0" t="s">
-        <x:v>342</x:v>
+        <x:v>343</x:v>
       </x:c>
       <x:c r="D110" s="0" t="s">
         <x:v>15</x:v>
@@ -3876,18 +4103,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F110" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G110" s="0" t="s">
-        <x:v>343</x:v>
+        <x:v>344</x:v>
       </x:c>
     </x:row>
     <x:row r="111" spans="1:7">
       <x:c r="B111" s="0" t="s">
-        <x:v>344</x:v>
+        <x:v>345</x:v>
       </x:c>
       <x:c r="C111" s="0" t="s">
-        <x:v>345</x:v>
+        <x:v>346</x:v>
       </x:c>
       <x:c r="D111" s="0" t="s">
         <x:v>15</x:v>
@@ -3896,38 +4123,38 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F111" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G111" s="0" t="s">
-        <x:v>346</x:v>
+        <x:v>347</x:v>
       </x:c>
     </x:row>
     <x:row r="112" spans="1:7">
       <x:c r="B112" s="0" t="s">
-        <x:v>347</x:v>
+        <x:v>348</x:v>
       </x:c>
       <x:c r="C112" s="0" t="s">
-        <x:v>348</x:v>
+        <x:v>349</x:v>
       </x:c>
       <x:c r="D112" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E112" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F112" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G112" s="0" t="s">
-        <x:v>349</x:v>
+        <x:v>350</x:v>
       </x:c>
     </x:row>
     <x:row r="113" spans="1:7">
       <x:c r="B113" s="0" t="s">
-        <x:v>350</x:v>
+        <x:v>351</x:v>
       </x:c>
       <x:c r="C113" s="0" t="s">
-        <x:v>351</x:v>
+        <x:v>352</x:v>
       </x:c>
       <x:c r="D113" s="0" t="s">
         <x:v>9</x:v>
@@ -3939,55 +4166,55 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G113" s="0" t="s">
-        <x:v>352</x:v>
+        <x:v>353</x:v>
       </x:c>
     </x:row>
     <x:row r="114" spans="1:7">
       <x:c r="B114" s="0" t="s">
-        <x:v>353</x:v>
+        <x:v>354</x:v>
       </x:c>
       <x:c r="C114" s="0" t="s">
-        <x:v>354</x:v>
+        <x:v>355</x:v>
       </x:c>
       <x:c r="D114" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E114" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F114" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G114" s="0" t="s">
-        <x:v>355</x:v>
+        <x:v>356</x:v>
       </x:c>
     </x:row>
     <x:row r="115" spans="1:7">
       <x:c r="B115" s="0" t="s">
-        <x:v>356</x:v>
+        <x:v>357</x:v>
       </x:c>
       <x:c r="C115" s="0" t="s">
-        <x:v>357</x:v>
+        <x:v>358</x:v>
       </x:c>
       <x:c r="D115" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E115" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F115" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G115" s="0" t="s">
-        <x:v>358</x:v>
+        <x:v>359</x:v>
       </x:c>
     </x:row>
     <x:row r="116" spans="1:7">
       <x:c r="B116" s="0" t="s">
-        <x:v>359</x:v>
+        <x:v>360</x:v>
       </x:c>
       <x:c r="C116" s="0" t="s">
-        <x:v>360</x:v>
+        <x:v>361</x:v>
       </x:c>
       <x:c r="D116" s="0" t="s">
         <x:v>9</x:v>
@@ -3999,15 +4226,15 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G116" s="0" t="s">
-        <x:v>361</x:v>
+        <x:v>362</x:v>
       </x:c>
     </x:row>
     <x:row r="117" spans="1:7">
       <x:c r="B117" s="0" t="s">
-        <x:v>362</x:v>
+        <x:v>363</x:v>
       </x:c>
       <x:c r="C117" s="0" t="s">
-        <x:v>363</x:v>
+        <x:v>364</x:v>
       </x:c>
       <x:c r="D117" s="0" t="s">
         <x:v>15</x:v>
@@ -4016,78 +4243,78 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F117" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G117" s="0" t="s">
-        <x:v>364</x:v>
+        <x:v>365</x:v>
       </x:c>
     </x:row>
     <x:row r="118" spans="1:7">
       <x:c r="B118" s="0" t="s">
-        <x:v>365</x:v>
+        <x:v>366</x:v>
       </x:c>
       <x:c r="C118" s="0" t="s">
-        <x:v>366</x:v>
+        <x:v>367</x:v>
       </x:c>
       <x:c r="D118" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E118" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F118" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G118" s="0" t="s">
-        <x:v>367</x:v>
+        <x:v>368</x:v>
       </x:c>
     </x:row>
     <x:row r="119" spans="1:7">
       <x:c r="B119" s="0" t="s">
-        <x:v>368</x:v>
+        <x:v>369</x:v>
       </x:c>
       <x:c r="C119" s="0" t="s">
-        <x:v>369</x:v>
+        <x:v>370</x:v>
       </x:c>
       <x:c r="D119" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E119" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F119" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G119" s="0" t="s">
-        <x:v>370</x:v>
+        <x:v>371</x:v>
       </x:c>
     </x:row>
     <x:row r="120" spans="1:7">
       <x:c r="B120" s="0" t="s">
-        <x:v>371</x:v>
+        <x:v>372</x:v>
       </x:c>
       <x:c r="C120" s="0" t="s">
-        <x:v>372</x:v>
+        <x:v>373</x:v>
       </x:c>
       <x:c r="D120" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E120" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F120" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G120" s="0" t="s">
-        <x:v>373</x:v>
+        <x:v>374</x:v>
       </x:c>
     </x:row>
     <x:row r="121" spans="1:7">
       <x:c r="B121" s="0" t="s">
-        <x:v>374</x:v>
+        <x:v>375</x:v>
       </x:c>
       <x:c r="C121" s="0" t="s">
-        <x:v>375</x:v>
+        <x:v>376</x:v>
       </x:c>
       <x:c r="D121" s="0" t="s">
         <x:v>15</x:v>
@@ -4096,18 +4323,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F121" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G121" s="0" t="s">
-        <x:v>376</x:v>
+        <x:v>377</x:v>
       </x:c>
     </x:row>
     <x:row r="122" spans="1:7">
       <x:c r="B122" s="0" t="s">
-        <x:v>377</x:v>
+        <x:v>378</x:v>
       </x:c>
       <x:c r="C122" s="0" t="s">
-        <x:v>378</x:v>
+        <x:v>379</x:v>
       </x:c>
       <x:c r="D122" s="0" t="s">
         <x:v>15</x:v>
@@ -4116,38 +4343,38 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F122" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G122" s="0" t="s">
-        <x:v>379</x:v>
+        <x:v>380</x:v>
       </x:c>
     </x:row>
     <x:row r="123" spans="1:7">
       <x:c r="B123" s="0" t="s">
-        <x:v>380</x:v>
+        <x:v>381</x:v>
       </x:c>
       <x:c r="C123" s="0" t="s">
-        <x:v>381</x:v>
+        <x:v>382</x:v>
       </x:c>
       <x:c r="D123" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E123" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F123" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G123" s="0" t="s">
-        <x:v>382</x:v>
+        <x:v>383</x:v>
       </x:c>
     </x:row>
     <x:row r="124" spans="1:7">
       <x:c r="B124" s="0" t="s">
-        <x:v>383</x:v>
+        <x:v>384</x:v>
       </x:c>
       <x:c r="C124" s="0" t="s">
-        <x:v>384</x:v>
+        <x:v>385</x:v>
       </x:c>
       <x:c r="D124" s="0" t="s">
         <x:v>15</x:v>
@@ -4156,18 +4383,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F124" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G124" s="0" t="s">
-        <x:v>385</x:v>
+        <x:v>386</x:v>
       </x:c>
     </x:row>
     <x:row r="125" spans="1:7">
       <x:c r="B125" s="0" t="s">
-        <x:v>386</x:v>
+        <x:v>387</x:v>
       </x:c>
       <x:c r="C125" s="0" t="s">
-        <x:v>387</x:v>
+        <x:v>388</x:v>
       </x:c>
       <x:c r="D125" s="0" t="s">
         <x:v>9</x:v>
@@ -4179,15 +4406,15 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G125" s="0" t="s">
-        <x:v>388</x:v>
+        <x:v>389</x:v>
       </x:c>
     </x:row>
     <x:row r="126" spans="1:7">
       <x:c r="B126" s="0" t="s">
-        <x:v>389</x:v>
+        <x:v>390</x:v>
       </x:c>
       <x:c r="C126" s="0" t="s">
-        <x:v>390</x:v>
+        <x:v>391</x:v>
       </x:c>
       <x:c r="D126" s="0" t="s">
         <x:v>15</x:v>
@@ -4196,18 +4423,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F126" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G126" s="0" t="s">
-        <x:v>391</x:v>
+        <x:v>392</x:v>
       </x:c>
     </x:row>
     <x:row r="127" spans="1:7">
       <x:c r="B127" s="0" t="s">
-        <x:v>392</x:v>
+        <x:v>393</x:v>
       </x:c>
       <x:c r="C127" s="0" t="s">
-        <x:v>393</x:v>
+        <x:v>394</x:v>
       </x:c>
       <x:c r="D127" s="0" t="s">
         <x:v>15</x:v>
@@ -4216,38 +4443,38 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F127" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G127" s="0" t="s">
-        <x:v>394</x:v>
+        <x:v>395</x:v>
       </x:c>
     </x:row>
     <x:row r="128" spans="1:7">
       <x:c r="B128" s="0" t="s">
-        <x:v>395</x:v>
+        <x:v>396</x:v>
       </x:c>
       <x:c r="C128" s="0" t="s">
-        <x:v>396</x:v>
+        <x:v>397</x:v>
       </x:c>
       <x:c r="D128" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="E128" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F128" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G128" s="0" t="s">
-        <x:v>397</x:v>
+        <x:v>398</x:v>
       </x:c>
     </x:row>
     <x:row r="129" spans="1:7">
       <x:c r="B129" s="0" t="s">
-        <x:v>398</x:v>
+        <x:v>399</x:v>
       </x:c>
       <x:c r="C129" s="0" t="s">
-        <x:v>399</x:v>
+        <x:v>400</x:v>
       </x:c>
       <x:c r="D129" s="0" t="s">
         <x:v>15</x:v>
@@ -4256,18 +4483,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F129" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G129" s="0" t="s">
-        <x:v>400</x:v>
+        <x:v>401</x:v>
       </x:c>
     </x:row>
     <x:row r="130" spans="1:7">
       <x:c r="B130" s="0" t="s">
-        <x:v>401</x:v>
+        <x:v>402</x:v>
       </x:c>
       <x:c r="C130" s="0" t="s">
-        <x:v>402</x:v>
+        <x:v>403</x:v>
       </x:c>
       <x:c r="D130" s="0" t="s">
         <x:v>15</x:v>
@@ -4276,18 +4503,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F130" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G130" s="0" t="s">
-        <x:v>403</x:v>
+        <x:v>404</x:v>
       </x:c>
     </x:row>
     <x:row r="131" spans="1:7">
       <x:c r="B131" s="0" t="s">
-        <x:v>404</x:v>
+        <x:v>405</x:v>
       </x:c>
       <x:c r="C131" s="0" t="s">
-        <x:v>405</x:v>
+        <x:v>406</x:v>
       </x:c>
       <x:c r="D131" s="0" t="s">
         <x:v>15</x:v>
@@ -4296,18 +4523,18 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F131" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G131" s="0" t="s">
-        <x:v>406</x:v>
+        <x:v>407</x:v>
       </x:c>
     </x:row>
     <x:row r="132" spans="1:7">
       <x:c r="B132" s="0" t="s">
-        <x:v>407</x:v>
+        <x:v>408</x:v>
       </x:c>
       <x:c r="C132" s="0" t="s">
-        <x:v>408</x:v>
+        <x:v>409</x:v>
       </x:c>
       <x:c r="D132" s="0" t="s">
         <x:v>15</x:v>
@@ -4316,58 +4543,58 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F132" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G132" s="0" t="s">
-        <x:v>409</x:v>
+        <x:v>410</x:v>
       </x:c>
     </x:row>
     <x:row r="133" spans="1:7">
       <x:c r="B133" s="0" t="s">
-        <x:v>410</x:v>
+        <x:v>411</x:v>
       </x:c>
       <x:c r="C133" s="0" t="s">
-        <x:v>411</x:v>
+        <x:v>412</x:v>
       </x:c>
       <x:c r="D133" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E133" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F133" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G133" s="0" t="s">
-        <x:v>292</x:v>
+        <x:v>293</x:v>
       </x:c>
     </x:row>
     <x:row r="134" spans="1:7">
       <x:c r="B134" s="0" t="s">
-        <x:v>412</x:v>
+        <x:v>413</x:v>
       </x:c>
       <x:c r="C134" s="0" t="s">
-        <x:v>413</x:v>
+        <x:v>414</x:v>
       </x:c>
       <x:c r="D134" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E134" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F134" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G134" s="0" t="s">
-        <x:v>414</x:v>
+        <x:v>415</x:v>
       </x:c>
     </x:row>
     <x:row r="135" spans="1:7">
       <x:c r="B135" s="0" t="s">
-        <x:v>415</x:v>
+        <x:v>416</x:v>
       </x:c>
       <x:c r="C135" s="0" t="s">
-        <x:v>416</x:v>
+        <x:v>417</x:v>
       </x:c>
       <x:c r="D135" s="0" t="s">
         <x:v>9</x:v>
@@ -4379,55 +4606,55 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G135" s="0" t="s">
-        <x:v>417</x:v>
+        <x:v>418</x:v>
       </x:c>
     </x:row>
     <x:row r="136" spans="1:7">
       <x:c r="B136" s="0" t="s">
-        <x:v>418</x:v>
+        <x:v>419</x:v>
       </x:c>
       <x:c r="C136" s="0" t="s">
-        <x:v>419</x:v>
+        <x:v>420</x:v>
       </x:c>
       <x:c r="D136" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E136" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F136" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G136" s="0" t="s">
-        <x:v>420</x:v>
+        <x:v>421</x:v>
       </x:c>
     </x:row>
     <x:row r="137" spans="1:7">
       <x:c r="B137" s="0" t="s">
-        <x:v>421</x:v>
+        <x:v>422</x:v>
       </x:c>
       <x:c r="C137" s="0" t="s">
-        <x:v>422</x:v>
+        <x:v>423</x:v>
       </x:c>
       <x:c r="D137" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E137" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F137" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G137" s="0" t="s">
-        <x:v>423</x:v>
+        <x:v>424</x:v>
       </x:c>
     </x:row>
     <x:row r="138" spans="1:7">
       <x:c r="B138" s="0" t="s">
-        <x:v>424</x:v>
+        <x:v>425</x:v>
       </x:c>
       <x:c r="C138" s="0" t="s">
-        <x:v>425</x:v>
+        <x:v>426</x:v>
       </x:c>
       <x:c r="D138" s="0" t="s">
         <x:v>15</x:v>
@@ -4436,38 +4663,38 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F138" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G138" s="0" t="s">
-        <x:v>426</x:v>
+        <x:v>427</x:v>
       </x:c>
     </x:row>
     <x:row r="139" spans="1:7">
       <x:c r="B139" s="0" t="s">
-        <x:v>427</x:v>
+        <x:v>428</x:v>
       </x:c>
       <x:c r="C139" s="0" t="s">
-        <x:v>428</x:v>
+        <x:v>429</x:v>
       </x:c>
       <x:c r="D139" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E139" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F139" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G139" s="0" t="s">
-        <x:v>429</x:v>
+        <x:v>430</x:v>
       </x:c>
     </x:row>
     <x:row r="140" spans="1:7">
       <x:c r="B140" s="0" t="s">
-        <x:v>430</x:v>
+        <x:v>431</x:v>
       </x:c>
       <x:c r="C140" s="0" t="s">
-        <x:v>431</x:v>
+        <x:v>432</x:v>
       </x:c>
       <x:c r="D140" s="0" t="s">
         <x:v>9</x:v>
@@ -4479,7 +4706,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="G140" s="0" t="s">
-        <x:v>432</x:v>
+        <x:v>433</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -4491,18 +4718,18 @@
 </x:worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:I21"/>
+  <x:dimension ref="A1:J21"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:9">
+    <x:row r="1" spans="1:10">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -4522,16 +4749,19 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="G1" s="0" t="s">
-        <x:v>433</x:v>
+        <x:v>434</x:v>
       </x:c>
       <x:c r="H1" s="0" t="s">
-        <x:v>434</x:v>
+        <x:v>435</x:v>
       </x:c>
       <x:c r="I1" s="0" t="s">
-        <x:v>435</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:9">
+        <x:v>436</x:v>
+      </x:c>
+      <x:c r="J1" s="0" t="s">
+        <x:v>437</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:10">
       <x:c r="B2" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
@@ -4548,13 +4778,417 @@
         <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:9">
+    <x:row r="3" spans="1:10">
       <x:c r="B3" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:10">
+      <x:c r="B4" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:10">
+      <x:c r="B5" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:10">
+      <x:c r="B6" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:10">
+      <x:c r="B7" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:10">
+      <x:c r="B8" s="0" t="s">
+        <x:v>147</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:10">
+      <x:c r="B9" s="0" t="s">
+        <x:v>255</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:10">
+      <x:c r="B10" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:10">
+      <x:c r="B11" s="0" t="s">
+        <x:v>297</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>298</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:10">
+      <x:c r="B12" s="0" t="s">
+        <x:v>303</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>304</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:10">
+      <x:c r="B13" s="0" t="s">
+        <x:v>321</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>322</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:10">
+      <x:c r="B14" s="0" t="s">
+        <x:v>327</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>328</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:10">
+      <x:c r="B15" s="0" t="s">
+        <x:v>333</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>334</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:10">
+      <x:c r="B16" s="0" t="s">
+        <x:v>336</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>337</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F16" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:10">
+      <x:c r="B17" s="0" t="s">
+        <x:v>351</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>352</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:10">
+      <x:c r="B18" s="0" t="s">
+        <x:v>360</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>361</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:10">
+      <x:c r="B19" s="0" t="s">
+        <x:v>387</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>388</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F19" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:10">
+      <x:c r="B20" s="0" t="s">
+        <x:v>416</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>417</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:10">
+      <x:c r="B21" s="0" t="s">
+        <x:v>431</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>432</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F21" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:J21"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:10">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="0" t="s">
+        <x:v>434</x:v>
+      </x:c>
+      <x:c r="H1" s="0" t="s">
+        <x:v>435</x:v>
+      </x:c>
+      <x:c r="I1" s="0" t="s">
+        <x:v>436</x:v>
+      </x:c>
+      <x:c r="J1" s="0" t="s">
+        <x:v>437</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:10">
+      <x:c r="B2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>438</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>439</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="s">
+        <x:v>440</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="s">
+        <x:v>441</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:10">
+      <x:c r="B3" s="0" t="s">
         <x:v>76</x:v>
       </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
@@ -4564,13 +5198,25 @@
       <x:c r="F3" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="4" spans="1:9">
+      <x:c r="G3" s="0" t="s">
+        <x:v>442</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="s">
+        <x:v>443</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
+        <x:v>444</x:v>
+      </x:c>
+      <x:c r="J3" s="0" t="s">
+        <x:v>445</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:10">
       <x:c r="B4" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
         <x:v>9</x:v>
@@ -4581,13 +5227,25 @@
       <x:c r="F4" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="5" spans="1:9">
+      <x:c r="G4" s="0" t="s">
+        <x:v>446</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
+        <x:v>447</x:v>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
+        <x:v>448</x:v>
+      </x:c>
+      <x:c r="J4" s="0" t="s">
+        <x:v>449</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:10">
       <x:c r="B5" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
         <x:v>9</x:v>
@@ -4598,13 +5256,25 @@
       <x:c r="F5" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="6" spans="1:9">
+      <x:c r="G5" s="0" t="s">
+        <x:v>450</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="s">
+        <x:v>451</x:v>
+      </x:c>
+      <x:c r="I5" s="0" t="s">
+        <x:v>452</x:v>
+      </x:c>
+      <x:c r="J5" s="0" t="s">
+        <x:v>453</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:10">
       <x:c r="B6" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
         <x:v>9</x:v>
@@ -4615,13 +5285,25 @@
       <x:c r="F6" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="7" spans="1:9">
+      <x:c r="G6" s="0" t="s">
+        <x:v>454</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
+        <x:v>455</x:v>
+      </x:c>
+      <x:c r="I6" s="0" t="s">
+        <x:v>452</x:v>
+      </x:c>
+      <x:c r="J6" s="0" t="s">
+        <x:v>456</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:10">
       <x:c r="B7" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
         <x:v>9</x:v>
@@ -4632,13 +5314,25 @@
       <x:c r="F7" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="8" spans="1:9">
+      <x:c r="G7" s="0" t="s">
+        <x:v>457</x:v>
+      </x:c>
+      <x:c r="H7" s="0" t="s">
+        <x:v>458</x:v>
+      </x:c>
+      <x:c r="I7" s="0" t="s">
+        <x:v>444</x:v>
+      </x:c>
+      <x:c r="J7" s="0" t="s">
+        <x:v>459</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:10">
       <x:c r="B8" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
         <x:v>9</x:v>
@@ -4649,13 +5343,25 @@
       <x:c r="F8" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="9" spans="1:9">
+      <x:c r="G8" s="0" t="s">
+        <x:v>460</x:v>
+      </x:c>
+      <x:c r="H8" s="0" t="s">
+        <x:v>461</x:v>
+      </x:c>
+      <x:c r="I8" s="0" t="s">
+        <x:v>452</x:v>
+      </x:c>
+      <x:c r="J8" s="0" t="s">
+        <x:v>462</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:10">
       <x:c r="B9" s="0" t="s">
-        <x:v>254</x:v>
+        <x:v>255</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
         <x:v>9</x:v>
@@ -4666,13 +5372,25 @@
       <x:c r="F9" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="10" spans="1:9">
+      <x:c r="G9" s="0" t="s">
+        <x:v>463</x:v>
+      </x:c>
+      <x:c r="H9" s="0" t="s">
+        <x:v>464</x:v>
+      </x:c>
+      <x:c r="I9" s="0" t="s">
+        <x:v>440</x:v>
+      </x:c>
+      <x:c r="J9" s="0" t="s">
+        <x:v>465</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:10">
       <x:c r="B10" s="0" t="s">
-        <x:v>260</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>261</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
         <x:v>9</x:v>
@@ -4683,13 +5401,25 @@
       <x:c r="F10" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="11" spans="1:9">
+      <x:c r="G10" s="0" t="s">
+        <x:v>466</x:v>
+      </x:c>
+      <x:c r="H10" s="0" t="s">
+        <x:v>467</x:v>
+      </x:c>
+      <x:c r="I10" s="0" t="s">
+        <x:v>452</x:v>
+      </x:c>
+      <x:c r="J10" s="0" t="s">
+        <x:v>468</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:10">
       <x:c r="B11" s="0" t="s">
-        <x:v>296</x:v>
+        <x:v>297</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>297</x:v>
+        <x:v>298</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
         <x:v>9</x:v>
@@ -4700,13 +5430,25 @@
       <x:c r="F11" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="12" spans="1:9">
+      <x:c r="G11" s="0" t="s">
+        <x:v>469</x:v>
+      </x:c>
+      <x:c r="H11" s="0" t="s">
+        <x:v>470</x:v>
+      </x:c>
+      <x:c r="I11" s="0" t="s">
+        <x:v>448</x:v>
+      </x:c>
+      <x:c r="J11" s="0" t="s">
+        <x:v>471</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:10">
       <x:c r="B12" s="0" t="s">
-        <x:v>302</x:v>
+        <x:v>303</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>303</x:v>
+        <x:v>304</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
         <x:v>9</x:v>
@@ -4717,13 +5459,25 @@
       <x:c r="F12" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="13" spans="1:9">
+      <x:c r="G12" s="0" t="s">
+        <x:v>472</x:v>
+      </x:c>
+      <x:c r="H12" s="0" t="s">
+        <x:v>473</x:v>
+      </x:c>
+      <x:c r="I12" s="0" t="s">
+        <x:v>448</x:v>
+      </x:c>
+      <x:c r="J12" s="0" t="s">
+        <x:v>474</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:10">
       <x:c r="B13" s="0" t="s">
-        <x:v>320</x:v>
+        <x:v>321</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>321</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
         <x:v>9</x:v>
@@ -4734,13 +5488,25 @@
       <x:c r="F13" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="14" spans="1:9">
+      <x:c r="G13" s="0" t="s">
+        <x:v>475</x:v>
+      </x:c>
+      <x:c r="H13" s="0" t="s">
+        <x:v>476</x:v>
+      </x:c>
+      <x:c r="I13" s="0" t="s">
+        <x:v>448</x:v>
+      </x:c>
+      <x:c r="J13" s="0" t="s">
+        <x:v>477</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:10">
       <x:c r="B14" s="0" t="s">
-        <x:v>326</x:v>
+        <x:v>327</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>327</x:v>
+        <x:v>328</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
         <x:v>9</x:v>
@@ -4751,13 +5517,25 @@
       <x:c r="F14" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="15" spans="1:9">
+      <x:c r="G14" s="0" t="s">
+        <x:v>478</x:v>
+      </x:c>
+      <x:c r="H14" s="0" t="s">
+        <x:v>479</x:v>
+      </x:c>
+      <x:c r="I14" s="0" t="s">
+        <x:v>444</x:v>
+      </x:c>
+      <x:c r="J14" s="0" t="s">
+        <x:v>480</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:10">
       <x:c r="B15" s="0" t="s">
-        <x:v>332</x:v>
+        <x:v>333</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>333</x:v>
+        <x:v>334</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
         <x:v>9</x:v>
@@ -4768,13 +5546,25 @@
       <x:c r="F15" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="16" spans="1:9">
+      <x:c r="G15" s="0" t="s">
+        <x:v>481</x:v>
+      </x:c>
+      <x:c r="H15" s="0" t="s">
+        <x:v>482</x:v>
+      </x:c>
+      <x:c r="I15" s="0" t="s">
+        <x:v>444</x:v>
+      </x:c>
+      <x:c r="J15" s="0" t="s">
+        <x:v>483</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:10">
       <x:c r="B16" s="0" t="s">
-        <x:v>335</x:v>
+        <x:v>336</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>336</x:v>
+        <x:v>337</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
         <x:v>9</x:v>
@@ -4785,13 +5575,25 @@
       <x:c r="F16" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="17" spans="1:9">
+      <x:c r="G16" s="0" t="s">
+        <x:v>484</x:v>
+      </x:c>
+      <x:c r="H16" s="0" t="s">
+        <x:v>485</x:v>
+      </x:c>
+      <x:c r="I16" s="0" t="s">
+        <x:v>448</x:v>
+      </x:c>
+      <x:c r="J16" s="0" t="s">
+        <x:v>486</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:10">
       <x:c r="B17" s="0" t="s">
-        <x:v>350</x:v>
+        <x:v>351</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>351</x:v>
+        <x:v>352</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
         <x:v>9</x:v>
@@ -4802,13 +5604,25 @@
       <x:c r="F17" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="18" spans="1:9">
+      <x:c r="G17" s="0" t="s">
+        <x:v>487</x:v>
+      </x:c>
+      <x:c r="H17" s="0" t="s">
+        <x:v>488</x:v>
+      </x:c>
+      <x:c r="I17" s="0" t="s">
+        <x:v>448</x:v>
+      </x:c>
+      <x:c r="J17" s="0" t="s">
+        <x:v>489</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:10">
       <x:c r="B18" s="0" t="s">
-        <x:v>359</x:v>
+        <x:v>360</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>360</x:v>
+        <x:v>361</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
         <x:v>9</x:v>
@@ -4819,13 +5633,25 @@
       <x:c r="F18" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="19" spans="1:9">
+      <x:c r="G18" s="0" t="s">
+        <x:v>490</x:v>
+      </x:c>
+      <x:c r="H18" s="0" t="s">
+        <x:v>491</x:v>
+      </x:c>
+      <x:c r="I18" s="0" t="s">
+        <x:v>440</x:v>
+      </x:c>
+      <x:c r="J18" s="0" t="s">
+        <x:v>492</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:10">
       <x:c r="B19" s="0" t="s">
-        <x:v>386</x:v>
+        <x:v>387</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>387</x:v>
+        <x:v>388</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
         <x:v>9</x:v>
@@ -4836,13 +5662,25 @@
       <x:c r="F19" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="20" spans="1:9">
+      <x:c r="G19" s="0" t="s">
+        <x:v>493</x:v>
+      </x:c>
+      <x:c r="H19" s="0" t="s">
+        <x:v>494</x:v>
+      </x:c>
+      <x:c r="I19" s="0" t="s">
+        <x:v>440</x:v>
+      </x:c>
+      <x:c r="J19" s="0" t="s">
+        <x:v>495</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:10">
       <x:c r="B20" s="0" t="s">
-        <x:v>415</x:v>
+        <x:v>416</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>416</x:v>
+        <x:v>417</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
         <x:v>9</x:v>
@@ -4853,13 +5691,25 @@
       <x:c r="F20" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="21" spans="1:9">
+      <x:c r="G20" s="0" t="s">
+        <x:v>496</x:v>
+      </x:c>
+      <x:c r="H20" s="0" t="s">
+        <x:v>497</x:v>
+      </x:c>
+      <x:c r="I20" s="0" t="s">
+        <x:v>440</x:v>
+      </x:c>
+      <x:c r="J20" s="0" t="s">
+        <x:v>498</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:10">
       <x:c r="B21" s="0" t="s">
-        <x:v>430</x:v>
+        <x:v>431</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>431</x:v>
+        <x:v>432</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
         <x:v>9</x:v>
@@ -4869,6 +5719,58 @@
       </x:c>
       <x:c r="F21" s="0" t="s">
         <x:v>11</x:v>
+      </x:c>
+      <x:c r="G21" s="0" t="s">
+        <x:v>499</x:v>
+      </x:c>
+      <x:c r="H21" s="0" t="s">
+        <x:v>500</x:v>
+      </x:c>
+      <x:c r="I21" s="0" t="s">
+        <x:v>452</x:v>
+      </x:c>
+      <x:c r="J21" s="0" t="s">
+        <x:v>501</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:F2"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:6">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>